<commit_message>
Push Desde Pc Rafa
</commit_message>
<xml_diff>
--- a/documentation/MODELO RELACIONAL.xlsx
+++ b/documentation/MODELO RELACIONAL.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Desktop\backlog-vortexbird\documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="18915" windowHeight="8265"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
   <si>
     <t>USUARIOS</t>
   </si>
@@ -74,6 +79,24 @@
   </si>
   <si>
     <t>pruebasCalidad</t>
+  </si>
+  <si>
+    <t>VERSIÓN</t>
+  </si>
+  <si>
+    <t>lineaBase</t>
+  </si>
+  <si>
+    <t>resumen</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>tipoIncidencia</t>
+  </si>
+  <si>
+    <t>estimacionOriginal</t>
   </si>
 </sst>
 </file>
@@ -162,6 +185,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -209,7 +235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -244,7 +270,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -453,16 +479,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G14"/>
+  <dimension ref="B2:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
@@ -622,6 +649,93 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>